<commit_message>
add features for any country
</commit_message>
<xml_diff>
--- a/HCP.xlsx
+++ b/HCP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BS365\Documents\python\glpg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEEB753-C45A-448D-8030-1BC0A888CACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5302287-2F15-4B6E-B598-6F773640BF3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2112" yWindow="2076" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>FIRST NAME</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>023 1234567</t>
+  </si>
+  <si>
+    <t>COUNTRY</t>
+  </si>
+  <si>
+    <t>NL</t>
   </si>
 </sst>
 </file>
@@ -382,21 +388,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="2" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,27 +410,30 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -432,10 +441,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>